<commit_message>
Removed Umls from project PLan
</commit_message>
<xml_diff>
--- a/Project Plan includes Tasks and Status/Detailed Project Plan.xlsx
+++ b/Project Plan includes Tasks and Status/Detailed Project Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
   <si>
     <t>Iteration</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Completed</t>
-  </si>
-  <si>
-    <t>Iteration 2</t>
   </si>
   <si>
     <t>Iteration 3</t>
@@ -264,7 +261,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
@@ -272,6 +269,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -579,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +598,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I45" si="0">IF(H2=0,"Done", "")</f>
+        <f t="shared" ref="I2:I35" si="0">IF(H2=0,"Done", "")</f>
         <v>Done</v>
       </c>
     </row>
@@ -787,7 +787,7 @@
         <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
@@ -811,7 +811,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
@@ -837,7 +837,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -861,7 +861,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2">
         <v>3</v>
@@ -887,7 +887,7 @@
         <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -911,7 +911,7 @@
         <v>23</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="2">
         <v>2</v>
@@ -987,7 +987,7 @@
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -1011,7 +1011,7 @@
         <v>23</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="2">
         <v>2</v>
@@ -1076,10 +1076,10 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="7"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
@@ -1091,7 +1091,7 @@
         <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
@@ -1121,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" s="2">
         <v>2</v>
@@ -1156,117 +1156,130 @@
         <v>20</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="D23" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4">
-        <v>3</v>
-      </c>
-      <c r="I23" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F24" s="4">
-        <v>1</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3</v>
+      </c>
       <c r="H24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Done</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F25" s="4">
-        <v>1</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="G25" s="4">
+        <v>2</v>
+      </c>
       <c r="H25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Done</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="4">
-        <v>1</v>
-      </c>
-      <c r="G26" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G26" s="4">
+        <v>3</v>
+      </c>
       <c r="H26" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
@@ -1274,10 +1287,10 @@
         <v>12</v>
       </c>
       <c r="F27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H27" s="4">
         <v>0</v>
@@ -1287,458 +1300,225 @@
         <v>Done</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F28" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="D29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="G29" s="4">
-        <v>2</v>
-      </c>
+      <c r="G29" s="4"/>
       <c r="H29" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" t="str">
         <f t="shared" si="0"/>
-        <v>Done</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+        <v/>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F30" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D31" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F31" s="4">
-        <v>3</v>
-      </c>
-      <c r="G31" s="4">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G31" s="4"/>
       <c r="H31" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="J31">
+        <f>SUM(F22:F31)</f>
+        <v>24</v>
+      </c>
+      <c r="K31">
+        <f>J31-SUM(H22:H31)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="4">
-        <v>1</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4">
-        <v>1</v>
+      <c r="A32" s="5">
+        <v>41596</v>
+      </c>
+      <c r="B32" s="6">
+        <v>3</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6">
+        <v>2</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6">
+        <v>2</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="J32" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="4">
-        <v>2</v>
-      </c>
-      <c r="G33" s="4">
-        <v>2</v>
-      </c>
-      <c r="H33" s="4">
-        <v>0</v>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6">
+        <v>15</v>
       </c>
       <c r="I33" t="str">
         <f t="shared" si="0"/>
-        <v>Done</v>
+        <v/>
+      </c>
+      <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4">
-        <v>1</v>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6">
+        <v>15</v>
+      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6">
+        <v>15</v>
       </c>
       <c r="I34" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="J34">
+        <f>SUM(F32:F34)</f>
+        <v>32</v>
+      </c>
+      <c r="K34">
+        <f>J34-SUM(H32:H34)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="4">
-        <v>3</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4">
-        <v>3</v>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35">
+        <f>SUM(F2:F34)</f>
+        <v>91</v>
+      </c>
+      <c r="H35">
+        <f>SUM(H2:H34)</f>
+        <v>49</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4">
-        <v>1</v>
-      </c>
-      <c r="I36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="4">
-        <v>2</v>
-      </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4">
-        <v>2</v>
-      </c>
-      <c r="I37" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="4">
-        <v>1</v>
-      </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4">
-        <v>1</v>
-      </c>
-      <c r="I38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="4">
-        <v>3</v>
-      </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4">
-        <v>3</v>
-      </c>
-      <c r="I39" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K39" s="7"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F40" s="4">
-        <v>1</v>
-      </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4">
-        <v>1</v>
-      </c>
-      <c r="I40" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J40" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F41" s="4">
-        <v>2</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4">
-        <v>2</v>
-      </c>
-      <c r="I41" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J41">
-        <f>SUM(F22:F41)</f>
-        <v>34</v>
-      </c>
-      <c r="K41">
-        <f>J41-SUM(H22:H41)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>41596</v>
-      </c>
-      <c r="B42" s="6">
-        <v>3</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6">
-        <v>2</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6">
-        <v>2</v>
-      </c>
-      <c r="I42" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K42" s="7"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6">
-        <v>15</v>
-      </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6">
-        <v>15</v>
-      </c>
-      <c r="I43" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J43" t="s">
-        <v>37</v>
-      </c>
-      <c r="K43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6">
-        <v>15</v>
-      </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6">
-        <v>15</v>
-      </c>
-      <c r="I44" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J44">
-        <f>SUM(F42:F44)</f>
-        <v>32</v>
-      </c>
-      <c r="K44">
-        <f>J44-SUM(H42:H44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45">
-        <f>SUM(F2:F44)</f>
-        <v>101</v>
-      </c>
-      <c r="H45">
-        <f>SUM(H2:H44)</f>
-        <v>59</v>
-      </c>
-      <c r="I45" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J32:K32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Plan for presentation
</commit_message>
<xml_diff>
--- a/Project Plan includes Tasks and Status/Detailed Project Plan.xlsx
+++ b/Project Plan includes Tasks and Status/Detailed Project Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="52">
   <si>
     <t>Iteration</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Iteration 2</t>
+  </si>
+  <si>
+    <t>Sprint Story Management</t>
+  </si>
+  <si>
+    <t>Sprint Story Creation</t>
   </si>
 </sst>
 </file>
@@ -272,13 +278,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -583,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I39" si="0">IF(H2=0,"Done", "")</f>
+        <f t="shared" ref="I2:I41" si="0">IF(H2=0,"Done", "")</f>
         <v>Done</v>
       </c>
     </row>
@@ -1080,11 +1086,11 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="J19" s="7" t="s">
+      <c r="J19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -1111,13 +1117,13 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1144,15 +1150,15 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="7">
         <f>SUM(F2:F21)</f>
         <v>35</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="7">
         <f>SUM(G2:G21)</f>
         <v>35</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="7">
         <f>SUM(H2:H21)</f>
         <v>0</v>
       </c>
@@ -1184,8 +1190,8 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
@@ -1206,12 +1212,12 @@
       <c r="H23" s="4">
         <v>0</v>
       </c>
-      <c r="I23" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>Done</v>
-      </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="I23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
@@ -1420,11 +1426,11 @@
         <f t="shared" si="0"/>
         <v>Done</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
@@ -1449,13 +1455,13 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K32" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1482,15 +1488,15 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J33" s="8">
+      <c r="J33" s="7">
         <f>SUM(F24:F33)</f>
         <v>22</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33" s="7">
         <f>SUM(G24:G33)</f>
         <v>20</v>
       </c>
-      <c r="L33" s="8">
+      <c r="L33" s="7">
         <f>SUM(H24:H33)</f>
         <v>5</v>
       </c>
@@ -1502,11 +1508,11 @@
       <c r="B34" s="6">
         <v>3</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>47</v>
       </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="6">
@@ -1520,11 +1526,11 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="6">
@@ -1538,104 +1544,140 @@
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="6" t="s">
-        <v>40</v>
+      <c r="C36" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E36" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="E36" s="10"/>
       <c r="F36" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6">
-        <v>2</v>
-      </c>
-      <c r="I36" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+      <c r="C37" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="D37" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="E37" s="10"/>
       <c r="F37" s="6">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6">
-        <v>15</v>
-      </c>
-      <c r="I37" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="A38" s="5"/>
       <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
+      <c r="C38" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="D38" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6">
+        <v>2</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6">
         <v>15</v>
       </c>
-      <c r="I38" t="str">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6">
+        <v>15</v>
+      </c>
+      <c r="I39" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J38" s="8">
-        <f>SUM(F36:F38)</f>
-        <v>32</v>
-      </c>
-      <c r="K38" s="8">
-        <f>SUM(G36:G38)</f>
-        <v>0</v>
-      </c>
-      <c r="L38" s="8">
-        <f>SUM(H36:H38)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+      <c r="J39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6">
+        <v>15</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6">
+        <v>15</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="J40" s="7">
+        <f>SUM(F34:F40)</f>
+        <v>44</v>
+      </c>
+      <c r="K40" s="7">
+        <f>SUM(G34:G40)</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="7">
+        <f>SUM(H34:H40)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>39</v>
       </c>
-      <c r="F39">
-        <f>SUM(F2:F38)</f>
-        <v>96</v>
-      </c>
-      <c r="H39">
-        <f>SUM(H2:H38)</f>
-        <v>40</v>
-      </c>
-      <c r="I39" t="str">
+      <c r="F41">
+        <f>SUM(F2:F40)</f>
+        <v>104</v>
+      </c>
+      <c r="H41">
+        <f>SUM(H2:H40)</f>
+        <v>48</v>
+      </c>
+      <c r="I41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1644,7 +1686,7 @@
   <mergeCells count="3">
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="J19:L19"/>
-    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="J38:L38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>